<commit_message>
sửa tên báo cáo
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Direct_Sales_Order_General.xlsx
+++ b/DMS/Templates/Report_Direct_Sales_Order_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8396D2-51A9-4C00-9B97-F0C8C4FCEA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCED6918-0382-44D7-ADA0-2587EC6BA3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>VAT</t>
   </si>
   <si>
-    <t>BÁO CÁO TỔNG HỢP BÁN HÀNG</t>
-  </si>
-  <si>
     <t>{{Start}}</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>{{ReportSalesOrderGenerals.SalesOrders.BuyerStoreStatusName}}</t>
+  </si>
+  <si>
+    <t>BÁO CÁO TỔNG HỢP BÁN HÀNG TRỰC TIẾP</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -600,13 +600,13 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="4"/>
     </row>
@@ -621,7 +621,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -658,34 +658,34 @@
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29.25" x14ac:dyDescent="0.25">
@@ -698,16 +698,16 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thêm số tiền giảm giá vào báo cáo tổng hợp bán hàng trực tiếp
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Direct_Sales_Order_General.xlsx
+++ b/DMS/Templates/Report_Direct_Sales_Order_General.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCED6918-0382-44D7-ADA0-2587EC6BA3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9205786D-2534-44F7-AE31-A040690909B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24480" yWindow="1092" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Chiết khấu</t>
   </si>
   <si>
-    <t>Doanh thu</t>
-  </si>
-  <si>
     <t>Tổng</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>{{Total.TotalDiscount}}</t>
   </si>
   <si>
-    <t>{{Total.TotalRevenue}}</t>
-  </si>
-  <si>
     <t>{{Total.SubTotal}}</t>
   </si>
   <si>
@@ -121,6 +115,30 @@
   </si>
   <si>
     <t>BÁO CÁO TỔNG HỢP BÁN HÀNG TRỰC TIẾP</t>
+  </si>
+  <si>
+    <t>Giảm giá</t>
+  </si>
+  <si>
+    <t>Tôgnr tiền</t>
+  </si>
+  <si>
+    <t>Tổng tiền sau thuế</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderGenerals.SalesOrders.TotalAfterTax}}</t>
+  </si>
+  <si>
+    <t>{{ReportSalesOrderGenerals.SalesOrders.PromotionValue}}</t>
+  </si>
+  <si>
+    <t>{{Total.PromotionValue}}</t>
+  </si>
+  <si>
+    <t>{{Total.TotalAfterTax}}</t>
+  </si>
+  <si>
+    <t>{{Total.Total}}</t>
   </si>
 </sst>
 </file>
@@ -192,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -215,11 +233,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -245,6 +300,9 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -257,7 +315,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -540,7 +604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -557,157 +621,179 @@
     <col min="7" max="7" width="17.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="15" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="10" max="12" width="16.140625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+    <row r="4" spans="1:12" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +802,7 @@
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>